<commit_message>
small adjustments to DD and DPE for EPICP to reflect dataset file
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_proc_elem/DPE_EPICP_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_proc_elem/DPE_EPICP_FRANZI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5342AECE-8A95-4B34-9C04-29A001822901}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9543C144-EB80-4814-8B6C-931848C1809E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="263">
   <si>
     <t>index</t>
   </si>
@@ -871,7 +871,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -879,7 +879,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1224,21 +1223,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="F119" sqref="F119:F120"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1283,21 +1283,24 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5" t="s">
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1307,6 +1310,9 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
       <c r="G3" t="s">
         <v>260</v>
       </c>
@@ -1320,7 +1326,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -1330,7 +1336,9 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>253</v>
       </c>
@@ -1347,7 +1355,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -1357,6 +1365,9 @@
       <c r="D5" t="s">
         <v>13</v>
       </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
       <c r="G5" t="s">
         <v>260</v>
       </c>
@@ -1370,7 +1381,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -1380,6 +1391,9 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
       <c r="G6" t="s">
         <v>260</v>
       </c>
@@ -1393,7 +1407,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -1403,6 +1417,9 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
       <c r="G7" t="s">
         <v>260</v>
       </c>
@@ -1416,7 +1433,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -1426,6 +1443,9 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
       <c r="G8" t="s">
         <v>260</v>
       </c>
@@ -1439,7 +1459,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -1449,6 +1469,9 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
       <c r="G9" t="s">
         <v>260</v>
       </c>
@@ -1462,7 +1485,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -1472,6 +1495,9 @@
       <c r="D10" t="s">
         <v>13</v>
       </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
       <c r="G10" t="s">
         <v>260</v>
       </c>
@@ -1485,7 +1511,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>30</v>
       </c>
@@ -1495,6 +1521,9 @@
       <c r="D11" t="s">
         <v>13</v>
       </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
       <c r="G11" t="s">
         <v>260</v>
       </c>
@@ -1508,7 +1537,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>32</v>
       </c>
@@ -1518,6 +1547,9 @@
       <c r="D12" t="s">
         <v>13</v>
       </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
       <c r="G12" t="s">
         <v>260</v>
       </c>
@@ -1531,7 +1563,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -1541,6 +1573,9 @@
       <c r="D13" t="s">
         <v>13</v>
       </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
       <c r="G13" t="s">
         <v>260</v>
       </c>
@@ -1554,7 +1589,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -1564,6 +1599,9 @@
       <c r="D14" t="s">
         <v>13</v>
       </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
       <c r="G14" t="s">
         <v>260</v>
       </c>
@@ -1577,7 +1615,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -1587,21 +1625,24 @@
       <c r="D15" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5" t="s">
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>40</v>
       </c>
@@ -1611,6 +1652,9 @@
       <c r="D16" t="s">
         <v>13</v>
       </c>
+      <c r="F16" t="s">
+        <v>40</v>
+      </c>
       <c r="G16" t="s">
         <v>260</v>
       </c>
@@ -1624,7 +1668,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>42</v>
       </c>
@@ -1634,6 +1678,9 @@
       <c r="D17" t="s">
         <v>13</v>
       </c>
+      <c r="F17" t="s">
+        <v>42</v>
+      </c>
       <c r="G17" t="s">
         <v>260</v>
       </c>
@@ -1647,7 +1694,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>44</v>
       </c>
@@ -1657,6 +1704,9 @@
       <c r="D18" t="s">
         <v>13</v>
       </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
       <c r="G18" t="s">
         <v>260</v>
       </c>
@@ -1670,7 +1720,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>46</v>
       </c>
@@ -1680,6 +1730,9 @@
       <c r="D19" t="s">
         <v>13</v>
       </c>
+      <c r="F19" t="s">
+        <v>46</v>
+      </c>
       <c r="G19" t="s">
         <v>260</v>
       </c>
@@ -1693,7 +1746,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>48</v>
       </c>
@@ -1703,6 +1756,9 @@
       <c r="D20" t="s">
         <v>13</v>
       </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
       <c r="G20" t="s">
         <v>260</v>
       </c>
@@ -1716,7 +1772,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>50</v>
       </c>
@@ -1726,7 +1782,9 @@
       <c r="D21" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G21" s="2" t="s">
         <v>253</v>
       </c>
@@ -1743,7 +1801,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>52</v>
       </c>
@@ -1753,6 +1811,9 @@
       <c r="D22" t="s">
         <v>13</v>
       </c>
+      <c r="F22" t="s">
+        <v>52</v>
+      </c>
       <c r="G22" t="s">
         <v>260</v>
       </c>
@@ -1766,7 +1827,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>54</v>
       </c>
@@ -1776,6 +1837,9 @@
       <c r="D23" t="s">
         <v>13</v>
       </c>
+      <c r="F23" t="s">
+        <v>54</v>
+      </c>
       <c r="G23" t="s">
         <v>260</v>
       </c>
@@ -1789,7 +1853,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>56</v>
       </c>
@@ -1799,6 +1863,9 @@
       <c r="D24" t="s">
         <v>13</v>
       </c>
+      <c r="F24" t="s">
+        <v>56</v>
+      </c>
       <c r="G24" t="s">
         <v>260</v>
       </c>
@@ -1812,7 +1879,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>58</v>
       </c>
@@ -1822,6 +1889,9 @@
       <c r="D25" t="s">
         <v>13</v>
       </c>
+      <c r="F25" t="s">
+        <v>58</v>
+      </c>
       <c r="G25" t="s">
         <v>260</v>
       </c>
@@ -1835,7 +1905,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>60</v>
       </c>
@@ -1845,6 +1915,9 @@
       <c r="D26" t="s">
         <v>13</v>
       </c>
+      <c r="F26" t="s">
+        <v>60</v>
+      </c>
       <c r="G26" t="s">
         <v>260</v>
       </c>
@@ -1858,7 +1931,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>62</v>
       </c>
@@ -1868,6 +1941,9 @@
       <c r="D27" t="s">
         <v>13</v>
       </c>
+      <c r="F27" t="s">
+        <v>62</v>
+      </c>
       <c r="G27" t="s">
         <v>260</v>
       </c>
@@ -1881,7 +1957,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>64</v>
       </c>
@@ -1891,6 +1967,9 @@
       <c r="D28" t="s">
         <v>13</v>
       </c>
+      <c r="F28" t="s">
+        <v>64</v>
+      </c>
       <c r="G28" t="s">
         <v>260</v>
       </c>
@@ -1904,7 +1983,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>66</v>
       </c>
@@ -1914,6 +1993,9 @@
       <c r="D29" t="s">
         <v>13</v>
       </c>
+      <c r="F29" t="s">
+        <v>66</v>
+      </c>
       <c r="G29" t="s">
         <v>260</v>
       </c>
@@ -1927,7 +2009,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>68</v>
       </c>
@@ -1937,6 +2019,9 @@
       <c r="D30" t="s">
         <v>13</v>
       </c>
+      <c r="F30" t="s">
+        <v>68</v>
+      </c>
       <c r="G30" t="s">
         <v>260</v>
       </c>
@@ -1950,7 +2035,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>70</v>
       </c>
@@ -1960,7 +2045,9 @@
       <c r="D31" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G31" s="2" t="s">
         <v>253</v>
       </c>
@@ -1977,7 +2064,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>72</v>
       </c>
@@ -1987,6 +2074,9 @@
       <c r="D32" t="s">
         <v>13</v>
       </c>
+      <c r="F32" t="s">
+        <v>72</v>
+      </c>
       <c r="G32" t="s">
         <v>260</v>
       </c>
@@ -2000,7 +2090,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>74</v>
       </c>
@@ -2010,6 +2100,9 @@
       <c r="D33" t="s">
         <v>13</v>
       </c>
+      <c r="F33" t="s">
+        <v>74</v>
+      </c>
       <c r="G33" t="s">
         <v>260</v>
       </c>
@@ -2023,7 +2116,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>76</v>
       </c>
@@ -2033,6 +2126,9 @@
       <c r="D34" t="s">
         <v>13</v>
       </c>
+      <c r="F34" t="s">
+        <v>76</v>
+      </c>
       <c r="G34" t="s">
         <v>260</v>
       </c>
@@ -2046,7 +2142,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>78</v>
       </c>
@@ -2056,6 +2152,9 @@
       <c r="D35" t="s">
         <v>13</v>
       </c>
+      <c r="F35" t="s">
+        <v>78</v>
+      </c>
       <c r="G35" t="s">
         <v>260</v>
       </c>
@@ -2069,7 +2168,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>80</v>
       </c>
@@ -2079,6 +2178,9 @@
       <c r="D36" t="s">
         <v>13</v>
       </c>
+      <c r="F36" t="s">
+        <v>80</v>
+      </c>
       <c r="G36" t="s">
         <v>260</v>
       </c>
@@ -2092,7 +2194,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>82</v>
       </c>
@@ -2102,6 +2204,9 @@
       <c r="D37" t="s">
         <v>13</v>
       </c>
+      <c r="F37" t="s">
+        <v>82</v>
+      </c>
       <c r="G37" t="s">
         <v>260</v>
       </c>
@@ -2115,7 +2220,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>84</v>
       </c>
@@ -2125,6 +2230,9 @@
       <c r="D38" t="s">
         <v>13</v>
       </c>
+      <c r="F38" t="s">
+        <v>84</v>
+      </c>
       <c r="G38" t="s">
         <v>260</v>
       </c>
@@ -2138,7 +2246,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>86</v>
       </c>
@@ -2148,6 +2256,9 @@
       <c r="D39" t="s">
         <v>13</v>
       </c>
+      <c r="F39" t="s">
+        <v>86</v>
+      </c>
       <c r="G39" t="s">
         <v>260</v>
       </c>
@@ -2161,7 +2272,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>88</v>
       </c>
@@ -2171,6 +2282,9 @@
       <c r="D40" t="s">
         <v>13</v>
       </c>
+      <c r="F40" t="s">
+        <v>88</v>
+      </c>
       <c r="G40" t="s">
         <v>260</v>
       </c>
@@ -2184,7 +2298,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>90</v>
       </c>
@@ -2194,6 +2308,9 @@
       <c r="D41" t="s">
         <v>13</v>
       </c>
+      <c r="F41" t="s">
+        <v>90</v>
+      </c>
       <c r="G41" t="s">
         <v>260</v>
       </c>
@@ -2207,7 +2324,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>92</v>
       </c>
@@ -2217,6 +2334,9 @@
       <c r="D42" t="s">
         <v>13</v>
       </c>
+      <c r="F42" t="s">
+        <v>92</v>
+      </c>
       <c r="G42" t="s">
         <v>260</v>
       </c>
@@ -2230,7 +2350,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>94</v>
       </c>
@@ -2240,6 +2360,9 @@
       <c r="D43" t="s">
         <v>13</v>
       </c>
+      <c r="F43" t="s">
+        <v>94</v>
+      </c>
       <c r="G43" t="s">
         <v>260</v>
       </c>
@@ -2253,7 +2376,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>96</v>
       </c>
@@ -2263,6 +2386,9 @@
       <c r="D44" t="s">
         <v>13</v>
       </c>
+      <c r="F44" t="s">
+        <v>96</v>
+      </c>
       <c r="G44" t="s">
         <v>260</v>
       </c>
@@ -2276,7 +2402,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>98</v>
       </c>
@@ -2286,6 +2412,9 @@
       <c r="D45" t="s">
         <v>13</v>
       </c>
+      <c r="F45" t="s">
+        <v>98</v>
+      </c>
       <c r="G45" t="s">
         <v>260</v>
       </c>
@@ -2299,7 +2428,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>100</v>
       </c>
@@ -2309,6 +2438,9 @@
       <c r="D46" t="s">
         <v>13</v>
       </c>
+      <c r="F46" t="s">
+        <v>100</v>
+      </c>
       <c r="G46" t="s">
         <v>260</v>
       </c>
@@ -2322,7 +2454,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>102</v>
       </c>
@@ -2332,6 +2464,9 @@
       <c r="D47" t="s">
         <v>13</v>
       </c>
+      <c r="F47" t="s">
+        <v>102</v>
+      </c>
       <c r="G47" t="s">
         <v>260</v>
       </c>
@@ -2345,7 +2480,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>104</v>
       </c>
@@ -2355,7 +2490,9 @@
       <c r="D48" t="s">
         <v>13</v>
       </c>
-      <c r="F48" s="3"/>
+      <c r="F48" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G48" s="2" t="s">
         <v>253</v>
       </c>
@@ -2372,7 +2509,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>106</v>
       </c>
@@ -2382,7 +2519,9 @@
       <c r="D49" t="s">
         <v>13</v>
       </c>
-      <c r="F49" s="3"/>
+      <c r="F49" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G49" s="2" t="s">
         <v>253</v>
       </c>
@@ -2399,7 +2538,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>108</v>
       </c>
@@ -2409,6 +2548,9 @@
       <c r="D50" t="s">
         <v>13</v>
       </c>
+      <c r="F50" t="s">
+        <v>108</v>
+      </c>
       <c r="G50" t="s">
         <v>260</v>
       </c>
@@ -2422,7 +2564,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>110</v>
       </c>
@@ -2432,6 +2574,9 @@
       <c r="D51" t="s">
         <v>13</v>
       </c>
+      <c r="F51" t="s">
+        <v>110</v>
+      </c>
       <c r="G51" t="s">
         <v>260</v>
       </c>
@@ -2445,7 +2590,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>112</v>
       </c>
@@ -2455,6 +2600,9 @@
       <c r="D52" t="s">
         <v>13</v>
       </c>
+      <c r="F52" t="s">
+        <v>112</v>
+      </c>
       <c r="G52" t="s">
         <v>260</v>
       </c>
@@ -2468,7 +2616,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>114</v>
       </c>
@@ -2478,7 +2626,9 @@
       <c r="D53" t="s">
         <v>13</v>
       </c>
-      <c r="F53" s="3"/>
+      <c r="F53" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G53" s="2" t="s">
         <v>253</v>
       </c>
@@ -2495,7 +2645,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>116</v>
       </c>
@@ -2505,7 +2655,9 @@
       <c r="D54" t="s">
         <v>13</v>
       </c>
-      <c r="F54" s="3"/>
+      <c r="F54" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G54" s="2" t="s">
         <v>253</v>
       </c>
@@ -2522,7 +2674,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>118</v>
       </c>
@@ -2532,7 +2684,9 @@
       <c r="D55" t="s">
         <v>13</v>
       </c>
-      <c r="F55" s="3"/>
+      <c r="F55" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G55" s="2" t="s">
         <v>253</v>
       </c>
@@ -2549,7 +2703,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>120</v>
       </c>
@@ -2559,6 +2713,9 @@
       <c r="D56" t="s">
         <v>13</v>
       </c>
+      <c r="F56" t="s">
+        <v>120</v>
+      </c>
       <c r="G56" t="s">
         <v>260</v>
       </c>
@@ -2572,7 +2729,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>122</v>
       </c>
@@ -2582,7 +2739,9 @@
       <c r="D57" t="s">
         <v>13</v>
       </c>
-      <c r="F57" s="3"/>
+      <c r="F57" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G57" s="2" t="s">
         <v>253</v>
       </c>
@@ -2599,7 +2758,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>124</v>
       </c>
@@ -2609,6 +2768,9 @@
       <c r="D58" t="s">
         <v>13</v>
       </c>
+      <c r="F58" t="s">
+        <v>124</v>
+      </c>
       <c r="G58" t="s">
         <v>260</v>
       </c>
@@ -2622,7 +2784,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>126</v>
       </c>
@@ -2632,6 +2794,9 @@
       <c r="D59" t="s">
         <v>13</v>
       </c>
+      <c r="F59" t="s">
+        <v>126</v>
+      </c>
       <c r="G59" t="s">
         <v>260</v>
       </c>
@@ -2645,7 +2810,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>128</v>
       </c>
@@ -2655,6 +2820,9 @@
       <c r="D60" t="s">
         <v>13</v>
       </c>
+      <c r="F60" t="s">
+        <v>128</v>
+      </c>
       <c r="G60" t="s">
         <v>260</v>
       </c>
@@ -2668,7 +2836,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>130</v>
       </c>
@@ -2678,6 +2846,9 @@
       <c r="D61" t="s">
         <v>13</v>
       </c>
+      <c r="F61" t="s">
+        <v>130</v>
+      </c>
       <c r="G61" t="s">
         <v>260</v>
       </c>
@@ -2691,7 +2862,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>132</v>
       </c>
@@ -2701,7 +2872,9 @@
       <c r="D62" t="s">
         <v>13</v>
       </c>
-      <c r="F62" s="3"/>
+      <c r="F62" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G62" s="2" t="s">
         <v>253</v>
       </c>
@@ -2718,7 +2891,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>134</v>
       </c>
@@ -2728,6 +2901,9 @@
       <c r="D63" t="s">
         <v>13</v>
       </c>
+      <c r="F63" t="s">
+        <v>134</v>
+      </c>
       <c r="G63" t="s">
         <v>260</v>
       </c>
@@ -2741,7 +2917,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>136</v>
       </c>
@@ -2751,6 +2927,9 @@
       <c r="D64" t="s">
         <v>13</v>
       </c>
+      <c r="F64" t="s">
+        <v>136</v>
+      </c>
       <c r="G64" t="s">
         <v>260</v>
       </c>
@@ -2764,7 +2943,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>138</v>
       </c>
@@ -2774,6 +2953,9 @@
       <c r="D65" t="s">
         <v>13</v>
       </c>
+      <c r="F65" t="s">
+        <v>138</v>
+      </c>
       <c r="G65" t="s">
         <v>260</v>
       </c>
@@ -2787,7 +2969,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>140</v>
       </c>
@@ -2797,6 +2979,9 @@
       <c r="D66" t="s">
         <v>13</v>
       </c>
+      <c r="F66" t="s">
+        <v>140</v>
+      </c>
       <c r="G66" t="s">
         <v>260</v>
       </c>
@@ -2810,7 +2995,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>142</v>
       </c>
@@ -2820,6 +3005,9 @@
       <c r="D67" t="s">
         <v>13</v>
       </c>
+      <c r="F67" t="s">
+        <v>142</v>
+      </c>
       <c r="G67" t="s">
         <v>260</v>
       </c>
@@ -2833,7 +3021,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>144</v>
       </c>
@@ -2843,6 +3031,9 @@
       <c r="D68" t="s">
         <v>13</v>
       </c>
+      <c r="F68" t="s">
+        <v>144</v>
+      </c>
       <c r="G68" t="s">
         <v>260</v>
       </c>
@@ -2856,7 +3047,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>146</v>
       </c>
@@ -2866,6 +3057,9 @@
       <c r="D69" t="s">
         <v>13</v>
       </c>
+      <c r="F69" t="s">
+        <v>146</v>
+      </c>
       <c r="G69" t="s">
         <v>260</v>
       </c>
@@ -2879,7 +3073,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>148</v>
       </c>
@@ -2889,6 +3083,9 @@
       <c r="D70" t="s">
         <v>13</v>
       </c>
+      <c r="F70" t="s">
+        <v>148</v>
+      </c>
       <c r="G70" t="s">
         <v>260</v>
       </c>
@@ -2902,7 +3099,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>150</v>
       </c>
@@ -2912,7 +3109,9 @@
       <c r="D71" t="s">
         <v>13</v>
       </c>
-      <c r="F71" s="3"/>
+      <c r="F71" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G71" s="2" t="s">
         <v>253</v>
       </c>
@@ -2929,7 +3128,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>152</v>
       </c>
@@ -2939,6 +3138,9 @@
       <c r="D72" t="s">
         <v>13</v>
       </c>
+      <c r="F72" t="s">
+        <v>152</v>
+      </c>
       <c r="G72" t="s">
         <v>260</v>
       </c>
@@ -2952,7 +3154,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>154</v>
       </c>
@@ -2962,6 +3164,9 @@
       <c r="D73" t="s">
         <v>13</v>
       </c>
+      <c r="F73" t="s">
+        <v>154</v>
+      </c>
       <c r="G73" t="s">
         <v>260</v>
       </c>
@@ -2975,7 +3180,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>156</v>
       </c>
@@ -2985,6 +3190,9 @@
       <c r="D74" t="s">
         <v>13</v>
       </c>
+      <c r="F74" t="s">
+        <v>156</v>
+      </c>
       <c r="G74" t="s">
         <v>260</v>
       </c>
@@ -2998,7 +3206,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>158</v>
       </c>
@@ -3008,6 +3216,9 @@
       <c r="D75" t="s">
         <v>13</v>
       </c>
+      <c r="F75" t="s">
+        <v>158</v>
+      </c>
       <c r="G75" t="s">
         <v>260</v>
       </c>
@@ -3021,7 +3232,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>160</v>
       </c>
@@ -3031,6 +3242,9 @@
       <c r="D76" t="s">
         <v>13</v>
       </c>
+      <c r="F76" t="s">
+        <v>160</v>
+      </c>
       <c r="G76" t="s">
         <v>260</v>
       </c>
@@ -3044,7 +3258,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>162</v>
       </c>
@@ -3054,7 +3268,9 @@
       <c r="D77" t="s">
         <v>13</v>
       </c>
-      <c r="F77" s="3"/>
+      <c r="F77" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G77" s="2" t="s">
         <v>253</v>
       </c>
@@ -3071,7 +3287,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>164</v>
       </c>
@@ -3081,6 +3297,9 @@
       <c r="D78" t="s">
         <v>13</v>
       </c>
+      <c r="F78" t="s">
+        <v>164</v>
+      </c>
       <c r="G78" t="s">
         <v>260</v>
       </c>
@@ -3094,7 +3313,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>166</v>
       </c>
@@ -3104,6 +3323,9 @@
       <c r="D79" t="s">
         <v>13</v>
       </c>
+      <c r="F79" t="s">
+        <v>166</v>
+      </c>
       <c r="G79" t="s">
         <v>260</v>
       </c>
@@ -3117,7 +3339,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>168</v>
       </c>
@@ -3127,7 +3349,9 @@
       <c r="D80" t="s">
         <v>13</v>
       </c>
-      <c r="F80" s="3"/>
+      <c r="F80" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G80" s="2" t="s">
         <v>253</v>
       </c>
@@ -3144,7 +3368,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>170</v>
       </c>
@@ -3154,7 +3378,9 @@
       <c r="D81" t="s">
         <v>13</v>
       </c>
-      <c r="F81" s="3"/>
+      <c r="F81" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G81" s="2" t="s">
         <v>253</v>
       </c>
@@ -3171,7 +3397,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>172</v>
       </c>
@@ -3181,6 +3407,9 @@
       <c r="D82" t="s">
         <v>13</v>
       </c>
+      <c r="F82" t="s">
+        <v>172</v>
+      </c>
       <c r="G82" t="s">
         <v>260</v>
       </c>
@@ -3194,7 +3423,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>174</v>
       </c>
@@ -3204,6 +3433,9 @@
       <c r="D83" t="s">
         <v>13</v>
       </c>
+      <c r="F83" t="s">
+        <v>174</v>
+      </c>
       <c r="G83" t="s">
         <v>260</v>
       </c>
@@ -3217,7 +3449,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>176</v>
       </c>
@@ -3227,6 +3459,9 @@
       <c r="D84" t="s">
         <v>13</v>
       </c>
+      <c r="F84" t="s">
+        <v>176</v>
+      </c>
       <c r="G84" t="s">
         <v>260</v>
       </c>
@@ -3240,7 +3475,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>178</v>
       </c>
@@ -3250,6 +3485,9 @@
       <c r="D85" t="s">
         <v>13</v>
       </c>
+      <c r="F85" t="s">
+        <v>178</v>
+      </c>
       <c r="G85" t="s">
         <v>260</v>
       </c>
@@ -3263,7 +3501,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>180</v>
       </c>
@@ -3273,6 +3511,9 @@
       <c r="D86" t="s">
         <v>13</v>
       </c>
+      <c r="F86" t="s">
+        <v>180</v>
+      </c>
       <c r="G86" t="s">
         <v>260</v>
       </c>
@@ -3286,7 +3527,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>182</v>
       </c>
@@ -3296,6 +3537,9 @@
       <c r="D87" t="s">
         <v>13</v>
       </c>
+      <c r="F87" t="s">
+        <v>182</v>
+      </c>
       <c r="G87" t="s">
         <v>260</v>
       </c>
@@ -3309,7 +3553,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>184</v>
       </c>
@@ -3319,6 +3563,9 @@
       <c r="D88" t="s">
         <v>13</v>
       </c>
+      <c r="F88" t="s">
+        <v>184</v>
+      </c>
       <c r="G88" t="s">
         <v>260</v>
       </c>
@@ -3332,7 +3579,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>186</v>
       </c>
@@ -3342,6 +3589,9 @@
       <c r="D89" t="s">
         <v>13</v>
       </c>
+      <c r="F89" t="s">
+        <v>186</v>
+      </c>
       <c r="G89" t="s">
         <v>260</v>
       </c>
@@ -3355,7 +3605,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>188</v>
       </c>
@@ -3365,6 +3615,9 @@
       <c r="D90" t="s">
         <v>13</v>
       </c>
+      <c r="F90" t="s">
+        <v>188</v>
+      </c>
       <c r="G90" t="s">
         <v>260</v>
       </c>
@@ -3378,7 +3631,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>190</v>
       </c>
@@ -3388,6 +3641,9 @@
       <c r="D91" t="s">
         <v>13</v>
       </c>
+      <c r="F91" t="s">
+        <v>190</v>
+      </c>
       <c r="G91" t="s">
         <v>260</v>
       </c>
@@ -3401,7 +3657,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>192</v>
       </c>
@@ -3411,6 +3667,9 @@
       <c r="D92" t="s">
         <v>13</v>
       </c>
+      <c r="F92" t="s">
+        <v>192</v>
+      </c>
       <c r="G92" t="s">
         <v>260</v>
       </c>
@@ -3424,7 +3683,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>194</v>
       </c>
@@ -3434,6 +3693,9 @@
       <c r="D93" t="s">
         <v>13</v>
       </c>
+      <c r="F93" t="s">
+        <v>194</v>
+      </c>
       <c r="G93" t="s">
         <v>260</v>
       </c>
@@ -3447,7 +3709,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>196</v>
       </c>
@@ -3457,6 +3719,9 @@
       <c r="D94" t="s">
         <v>13</v>
       </c>
+      <c r="F94" t="s">
+        <v>196</v>
+      </c>
       <c r="G94" t="s">
         <v>260</v>
       </c>
@@ -3470,7 +3735,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>198</v>
       </c>
@@ -3480,6 +3745,9 @@
       <c r="D95" t="s">
         <v>13</v>
       </c>
+      <c r="F95" t="s">
+        <v>198</v>
+      </c>
       <c r="G95" t="s">
         <v>260</v>
       </c>
@@ -3493,7 +3761,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>200</v>
       </c>
@@ -3503,6 +3771,9 @@
       <c r="D96" t="s">
         <v>13</v>
       </c>
+      <c r="F96" t="s">
+        <v>200</v>
+      </c>
       <c r="G96" t="s">
         <v>260</v>
       </c>
@@ -3516,7 +3787,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>202</v>
       </c>
@@ -3526,6 +3797,9 @@
       <c r="D97" t="s">
         <v>13</v>
       </c>
+      <c r="F97" t="s">
+        <v>202</v>
+      </c>
       <c r="G97" t="s">
         <v>260</v>
       </c>
@@ -3539,7 +3813,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>204</v>
       </c>
@@ -3549,6 +3823,9 @@
       <c r="D98" t="s">
         <v>13</v>
       </c>
+      <c r="F98" t="s">
+        <v>204</v>
+      </c>
       <c r="G98" t="s">
         <v>260</v>
       </c>
@@ -3562,7 +3839,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>206</v>
       </c>
@@ -3572,6 +3849,9 @@
       <c r="D99" t="s">
         <v>13</v>
       </c>
+      <c r="F99" t="s">
+        <v>206</v>
+      </c>
       <c r="G99" t="s">
         <v>260</v>
       </c>
@@ -3585,7 +3865,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>208</v>
       </c>
@@ -3595,6 +3875,9 @@
       <c r="D100" t="s">
         <v>13</v>
       </c>
+      <c r="F100" t="s">
+        <v>208</v>
+      </c>
       <c r="G100" t="s">
         <v>260</v>
       </c>
@@ -3608,7 +3891,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>210</v>
       </c>
@@ -3618,7 +3901,9 @@
       <c r="D101" t="s">
         <v>13</v>
       </c>
-      <c r="F101" s="3"/>
+      <c r="F101" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G101" s="2" t="s">
         <v>253</v>
       </c>
@@ -3635,7 +3920,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>212</v>
       </c>
@@ -3645,6 +3930,9 @@
       <c r="D102" t="s">
         <v>13</v>
       </c>
+      <c r="F102" t="s">
+        <v>212</v>
+      </c>
       <c r="G102" t="s">
         <v>260</v>
       </c>
@@ -3658,7 +3946,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>214</v>
       </c>
@@ -3668,6 +3956,9 @@
       <c r="D103" t="s">
         <v>13</v>
       </c>
+      <c r="F103" t="s">
+        <v>214</v>
+      </c>
       <c r="G103" t="s">
         <v>260</v>
       </c>
@@ -3681,7 +3972,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>216</v>
       </c>
@@ -3691,6 +3982,9 @@
       <c r="D104" t="s">
         <v>13</v>
       </c>
+      <c r="F104" t="s">
+        <v>216</v>
+      </c>
       <c r="G104" t="s">
         <v>260</v>
       </c>
@@ -3704,7 +3998,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>218</v>
       </c>
@@ -3714,6 +4008,9 @@
       <c r="D105" t="s">
         <v>13</v>
       </c>
+      <c r="F105" t="s">
+        <v>218</v>
+      </c>
       <c r="G105" t="s">
         <v>260</v>
       </c>
@@ -3727,7 +4024,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>220</v>
       </c>
@@ -3737,6 +4034,9 @@
       <c r="D106" t="s">
         <v>13</v>
       </c>
+      <c r="F106" t="s">
+        <v>220</v>
+      </c>
       <c r="G106" t="s">
         <v>260</v>
       </c>
@@ -3750,7 +4050,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>222</v>
       </c>
@@ -3760,7 +4060,9 @@
       <c r="D107" t="s">
         <v>13</v>
       </c>
-      <c r="F107" s="3"/>
+      <c r="F107" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G107" s="2" t="s">
         <v>253</v>
       </c>
@@ -3777,7 +4079,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>224</v>
       </c>
@@ -3787,7 +4089,9 @@
       <c r="D108" t="s">
         <v>13</v>
       </c>
-      <c r="F108" s="3"/>
+      <c r="F108" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G108" s="2" t="s">
         <v>253</v>
       </c>
@@ -3804,7 +4108,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>226</v>
       </c>
@@ -3814,6 +4118,9 @@
       <c r="D109" t="s">
         <v>13</v>
       </c>
+      <c r="F109" t="s">
+        <v>226</v>
+      </c>
       <c r="G109" t="s">
         <v>260</v>
       </c>
@@ -3827,7 +4134,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>228</v>
       </c>
@@ -3837,6 +4144,9 @@
       <c r="D110" t="s">
         <v>13</v>
       </c>
+      <c r="F110" t="s">
+        <v>228</v>
+      </c>
       <c r="G110" t="s">
         <v>260</v>
       </c>
@@ -3850,7 +4160,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>230</v>
       </c>
@@ -3860,6 +4170,9 @@
       <c r="D111" t="s">
         <v>13</v>
       </c>
+      <c r="F111" t="s">
+        <v>230</v>
+      </c>
       <c r="G111" t="s">
         <v>260</v>
       </c>
@@ -3873,7 +4186,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>232</v>
       </c>
@@ -3883,6 +4196,9 @@
       <c r="D112" t="s">
         <v>13</v>
       </c>
+      <c r="F112" t="s">
+        <v>232</v>
+      </c>
       <c r="G112" t="s">
         <v>260</v>
       </c>
@@ -3896,7 +4212,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>234</v>
       </c>
@@ -3906,6 +4222,9 @@
       <c r="D113" t="s">
         <v>13</v>
       </c>
+      <c r="F113" t="s">
+        <v>234</v>
+      </c>
       <c r="G113" t="s">
         <v>260</v>
       </c>
@@ -3919,7 +4238,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>236</v>
       </c>
@@ -3929,6 +4248,9 @@
       <c r="D114" t="s">
         <v>13</v>
       </c>
+      <c r="F114" t="s">
+        <v>236</v>
+      </c>
       <c r="G114" t="s">
         <v>260</v>
       </c>
@@ -3942,7 +4264,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="115" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>238</v>
       </c>
@@ -3952,6 +4274,9 @@
       <c r="D115" t="s">
         <v>13</v>
       </c>
+      <c r="F115" t="s">
+        <v>238</v>
+      </c>
       <c r="G115" t="s">
         <v>260</v>
       </c>
@@ -3965,7 +4290,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="116" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>240</v>
       </c>
@@ -3975,6 +4300,9 @@
       <c r="D116" t="s">
         <v>13</v>
       </c>
+      <c r="F116" t="s">
+        <v>240</v>
+      </c>
       <c r="G116" t="s">
         <v>260</v>
       </c>
@@ -3988,7 +4316,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="117" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>242</v>
       </c>
@@ -3998,6 +4326,9 @@
       <c r="D117" t="s">
         <v>13</v>
       </c>
+      <c r="F117" t="s">
+        <v>242</v>
+      </c>
       <c r="G117" t="s">
         <v>260</v>
       </c>
@@ -4011,7 +4342,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="118" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>244</v>
       </c>
@@ -4021,6 +4352,9 @@
       <c r="D118" t="s">
         <v>13</v>
       </c>
+      <c r="F118" t="s">
+        <v>244</v>
+      </c>
       <c r="G118" t="s">
         <v>260</v>
       </c>
@@ -4034,7 +4368,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="119" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>246</v>
       </c>
@@ -4044,7 +4378,9 @@
       <c r="D119" t="s">
         <v>13</v>
       </c>
-      <c r="F119" s="3"/>
+      <c r="F119" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G119" s="2" t="s">
         <v>253</v>
       </c>
@@ -4061,7 +4397,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="120" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>248</v>
       </c>
@@ -4071,7 +4407,9 @@
       <c r="D120" t="s">
         <v>13</v>
       </c>
-      <c r="F120" s="3"/>
+      <c r="F120" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="G120" s="2" t="s">
         <v>253</v>
       </c>
@@ -4088,7 +4426,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="121" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>250</v>
       </c>
@@ -4098,22 +4436,22 @@
       <c r="D121" t="s">
         <v>252</v>
       </c>
-      <c r="F121" s="4" t="s">
+      <c r="F121" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="G121" s="4" t="s">
+      <c r="G121" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="H121" s="4">
+      <c r="H121" s="3">
         <v>1</v>
       </c>
-      <c r="I121" s="4" t="s">
+      <c r="I121" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="J121" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="K121" s="4" t="s">
+      <c r="J121" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="K121" s="3" t="s">
         <v>259</v>
       </c>
     </row>

</xml_diff>